<commit_message>
Updated OCR app features and fixes
</commit_message>
<xml_diff>
--- a/data/reports/test_reports.xlsx
+++ b/data/reports/test_reports.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AK7"/>
+  <dimension ref="A1:AW11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -617,6 +617,66 @@
       <c r="AK1" s="1" t="inlineStr">
         <is>
           <t>Gamma Glutamyl Transferase</t>
+        </is>
+      </c>
+      <c r="AL1" s="1" t="inlineStr">
+        <is>
+          <t>Patient Name</t>
+        </is>
+      </c>
+      <c r="AM1" s="1" t="inlineStr">
+        <is>
+          <t>Patient Age</t>
+        </is>
+      </c>
+      <c r="AN1" s="1" t="inlineStr">
+        <is>
+          <t>Patient Gender</t>
+        </is>
+      </c>
+      <c r="AO1" s="1" t="inlineStr">
+        <is>
+          <t>Liver Size</t>
+        </is>
+      </c>
+      <c r="AP1" s="1" t="inlineStr">
+        <is>
+          <t>Gall Bladder Status</t>
+        </is>
+      </c>
+      <c r="AQ1" s="1" t="inlineStr">
+        <is>
+          <t>Spleen Size</t>
+        </is>
+      </c>
+      <c r="AR1" s="1" t="inlineStr">
+        <is>
+          <t>Pancreas Status</t>
+        </is>
+      </c>
+      <c r="AS1" s="1" t="inlineStr">
+        <is>
+          <t>Right Kidney Size</t>
+        </is>
+      </c>
+      <c r="AT1" s="1" t="inlineStr">
+        <is>
+          <t>Left Kidney Size</t>
+        </is>
+      </c>
+      <c r="AU1" s="1" t="inlineStr">
+        <is>
+          <t>Urinary Bladder Status</t>
+        </is>
+      </c>
+      <c r="AV1" s="1" t="inlineStr">
+        <is>
+          <t>Ultrasound Findings</t>
+        </is>
+      </c>
+      <c r="AW1" s="1" t="inlineStr">
+        <is>
+          <t>Ultrasound Impression</t>
         </is>
       </c>
     </row>
@@ -674,6 +734,18 @@
       <c r="AI2" t="inlineStr"/>
       <c r="AJ2" t="inlineStr"/>
       <c r="AK2" t="inlineStr"/>
+      <c r="AL2" t="inlineStr"/>
+      <c r="AM2" t="inlineStr"/>
+      <c r="AN2" t="inlineStr"/>
+      <c r="AO2" t="inlineStr"/>
+      <c r="AP2" t="inlineStr"/>
+      <c r="AQ2" t="inlineStr"/>
+      <c r="AR2" t="inlineStr"/>
+      <c r="AS2" t="inlineStr"/>
+      <c r="AT2" t="inlineStr"/>
+      <c r="AU2" t="inlineStr"/>
+      <c r="AV2" t="inlineStr"/>
+      <c r="AW2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -729,6 +801,18 @@
       <c r="AI3" t="inlineStr"/>
       <c r="AJ3" t="inlineStr"/>
       <c r="AK3" t="inlineStr"/>
+      <c r="AL3" t="inlineStr"/>
+      <c r="AM3" t="inlineStr"/>
+      <c r="AN3" t="inlineStr"/>
+      <c r="AO3" t="inlineStr"/>
+      <c r="AP3" t="inlineStr"/>
+      <c r="AQ3" t="inlineStr"/>
+      <c r="AR3" t="inlineStr"/>
+      <c r="AS3" t="inlineStr"/>
+      <c r="AT3" t="inlineStr"/>
+      <c r="AU3" t="inlineStr"/>
+      <c r="AV3" t="inlineStr"/>
+      <c r="AW3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -784,6 +868,18 @@
       <c r="AI4" t="inlineStr"/>
       <c r="AJ4" t="inlineStr"/>
       <c r="AK4" t="inlineStr"/>
+      <c r="AL4" t="inlineStr"/>
+      <c r="AM4" t="inlineStr"/>
+      <c r="AN4" t="inlineStr"/>
+      <c r="AO4" t="inlineStr"/>
+      <c r="AP4" t="inlineStr"/>
+      <c r="AQ4" t="inlineStr"/>
+      <c r="AR4" t="inlineStr"/>
+      <c r="AS4" t="inlineStr"/>
+      <c r="AT4" t="inlineStr"/>
+      <c r="AU4" t="inlineStr"/>
+      <c r="AV4" t="inlineStr"/>
+      <c r="AW4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -839,6 +935,18 @@
       <c r="AI5" t="inlineStr"/>
       <c r="AJ5" t="inlineStr"/>
       <c r="AK5" t="inlineStr"/>
+      <c r="AL5" t="inlineStr"/>
+      <c r="AM5" t="inlineStr"/>
+      <c r="AN5" t="inlineStr"/>
+      <c r="AO5" t="inlineStr"/>
+      <c r="AP5" t="inlineStr"/>
+      <c r="AQ5" t="inlineStr"/>
+      <c r="AR5" t="inlineStr"/>
+      <c r="AS5" t="inlineStr"/>
+      <c r="AT5" t="inlineStr"/>
+      <c r="AU5" t="inlineStr"/>
+      <c r="AV5" t="inlineStr"/>
+      <c r="AW5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -894,6 +1002,18 @@
       <c r="AI6" t="inlineStr"/>
       <c r="AJ6" t="inlineStr"/>
       <c r="AK6" t="inlineStr"/>
+      <c r="AL6" t="inlineStr"/>
+      <c r="AM6" t="inlineStr"/>
+      <c r="AN6" t="inlineStr"/>
+      <c r="AO6" t="inlineStr"/>
+      <c r="AP6" t="inlineStr"/>
+      <c r="AQ6" t="inlineStr"/>
+      <c r="AR6" t="inlineStr"/>
+      <c r="AS6" t="inlineStr"/>
+      <c r="AT6" t="inlineStr"/>
+      <c r="AU6" t="inlineStr"/>
+      <c r="AV6" t="inlineStr"/>
+      <c r="AW6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -993,6 +1113,396 @@
       <c r="AK7" t="n">
         <v>10</v>
       </c>
+      <c r="AL7" t="inlineStr"/>
+      <c r="AM7" t="inlineStr"/>
+      <c r="AN7" t="inlineStr"/>
+      <c r="AO7" t="inlineStr"/>
+      <c r="AP7" t="inlineStr"/>
+      <c r="AQ7" t="inlineStr"/>
+      <c r="AR7" t="inlineStr"/>
+      <c r="AS7" t="inlineStr"/>
+      <c r="AT7" t="inlineStr"/>
+      <c r="AU7" t="inlineStr"/>
+      <c r="AV7" t="inlineStr"/>
+      <c r="AW7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2025-12-27</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Liver Function Test (LFT)</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>11.3</v>
+      </c>
+      <c r="D8" t="n">
+        <v>4.45</v>
+      </c>
+      <c r="E8" t="n">
+        <v>10.54</v>
+      </c>
+      <c r="F8" t="n">
+        <v>416</v>
+      </c>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="n">
+        <v>13</v>
+      </c>
+      <c r="J8" t="n">
+        <v>9</v>
+      </c>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="O8" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="P8" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>34</v>
+      </c>
+      <c r="R8" t="n">
+        <v>5</v>
+      </c>
+      <c r="S8" t="n">
+        <v>219</v>
+      </c>
+      <c r="T8" t="inlineStr"/>
+      <c r="U8" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="V8" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="W8" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="X8" t="n">
+        <v>34.7</v>
+      </c>
+      <c r="Y8" t="n">
+        <v>78</v>
+      </c>
+      <c r="Z8" t="n">
+        <v>25.4</v>
+      </c>
+      <c r="AA8" t="n">
+        <v>32</v>
+      </c>
+      <c r="AB8" t="n">
+        <v>12</v>
+      </c>
+      <c r="AC8" t="n">
+        <v>8.199999999999999</v>
+      </c>
+      <c r="AD8" t="inlineStr"/>
+      <c r="AE8" t="inlineStr"/>
+      <c r="AF8" t="inlineStr"/>
+      <c r="AG8" t="n">
+        <v>26</v>
+      </c>
+      <c r="AH8" t="n">
+        <v>79</v>
+      </c>
+      <c r="AI8" t="n">
+        <v>2</v>
+      </c>
+      <c r="AJ8" t="n">
+        <v>2</v>
+      </c>
+      <c r="AK8" t="n">
+        <v>10</v>
+      </c>
+      <c r="AL8" t="inlineStr"/>
+      <c r="AM8" t="inlineStr"/>
+      <c r="AN8" t="inlineStr"/>
+      <c r="AO8" t="inlineStr"/>
+      <c r="AP8" t="inlineStr"/>
+      <c r="AQ8" t="inlineStr"/>
+      <c r="AR8" t="inlineStr"/>
+      <c r="AS8" t="inlineStr"/>
+      <c r="AT8" t="inlineStr"/>
+      <c r="AU8" t="inlineStr"/>
+      <c r="AV8" t="inlineStr"/>
+      <c r="AW8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2025-12-28</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Vitals Check</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr"/>
+      <c r="O9" t="inlineStr"/>
+      <c r="P9" t="inlineStr"/>
+      <c r="Q9" t="inlineStr"/>
+      <c r="R9" t="inlineStr"/>
+      <c r="S9" t="inlineStr"/>
+      <c r="T9" t="inlineStr"/>
+      <c r="U9" t="inlineStr"/>
+      <c r="V9" t="inlineStr"/>
+      <c r="W9" t="inlineStr"/>
+      <c r="X9" t="inlineStr"/>
+      <c r="Y9" t="inlineStr"/>
+      <c r="Z9" t="inlineStr"/>
+      <c r="AA9" t="inlineStr"/>
+      <c r="AB9" t="inlineStr"/>
+      <c r="AC9" t="inlineStr"/>
+      <c r="AD9" t="inlineStr"/>
+      <c r="AE9" t="inlineStr"/>
+      <c r="AF9" t="inlineStr"/>
+      <c r="AG9" t="inlineStr"/>
+      <c r="AH9" t="inlineStr"/>
+      <c r="AI9" t="inlineStr"/>
+      <c r="AJ9" t="inlineStr"/>
+      <c r="AK9" t="inlineStr"/>
+      <c r="AL9" t="inlineStr"/>
+      <c r="AM9" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN9" t="inlineStr">
+        <is>
+          <t>Gender Leger</t>
+        </is>
+      </c>
+      <c r="AO9" t="n">
+        <v>68</v>
+      </c>
+      <c r="AP9" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="AQ9" t="n">
+        <v>48</v>
+      </c>
+      <c r="AR9" t="inlineStr"/>
+      <c r="AS9" t="inlineStr">
+        <is>
+          <t>43 x 19 mm</t>
+        </is>
+      </c>
+      <c r="AT9" t="inlineStr">
+        <is>
+          <t>48 x 22 mm</t>
+        </is>
+      </c>
+      <c r="AU9" t="inlineStr"/>
+      <c r="AV9" t="inlineStr">
+        <is>
+          <t>Acetabulum and iliac wing appear normal.
+Femoral head appears normal and cartilagenous.
+Central ossific nucleus not visualised in femoral head on either side.
+No joint effusion.
+No intramusclar fluid collection.
+Right angle Alpha - 61
+Beta - 56
+Left angle Alpha - 62
+Beta - 55
+No obvious e/o developmental dysplasia of hip.</t>
+        </is>
+      </c>
+      <c r="AW9" t="inlineStr">
+        <is>
+          <t>;
+Normal study. .</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2025-12-28</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Ultrasound Report</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr"/>
+      <c r="O10" t="inlineStr"/>
+      <c r="P10" t="inlineStr"/>
+      <c r="Q10" t="inlineStr"/>
+      <c r="R10" t="inlineStr"/>
+      <c r="S10" t="inlineStr"/>
+      <c r="T10" t="inlineStr"/>
+      <c r="U10" t="inlineStr"/>
+      <c r="V10" t="inlineStr"/>
+      <c r="W10" t="inlineStr"/>
+      <c r="X10" t="inlineStr"/>
+      <c r="Y10" t="inlineStr"/>
+      <c r="Z10" t="inlineStr"/>
+      <c r="AA10" t="inlineStr"/>
+      <c r="AB10" t="inlineStr"/>
+      <c r="AC10" t="inlineStr"/>
+      <c r="AD10" t="inlineStr"/>
+      <c r="AE10" t="inlineStr"/>
+      <c r="AF10" t="inlineStr"/>
+      <c r="AG10" t="inlineStr"/>
+      <c r="AH10" t="inlineStr"/>
+      <c r="AI10" t="inlineStr"/>
+      <c r="AJ10" t="inlineStr"/>
+      <c r="AK10" t="inlineStr"/>
+      <c r="AL10" t="inlineStr"/>
+      <c r="AM10" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN10" t="inlineStr">
+        <is>
+          <t>Gender Leger</t>
+        </is>
+      </c>
+      <c r="AO10" t="n">
+        <v>68</v>
+      </c>
+      <c r="AP10" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="AQ10" t="n">
+        <v>48</v>
+      </c>
+      <c r="AR10" t="inlineStr"/>
+      <c r="AS10" t="inlineStr">
+        <is>
+          <t>43 x 19 mm</t>
+        </is>
+      </c>
+      <c r="AT10" t="inlineStr">
+        <is>
+          <t>48 x 22 mm</t>
+        </is>
+      </c>
+      <c r="AU10" t="inlineStr"/>
+      <c r="AV10" t="inlineStr">
+        <is>
+          <t>Acetabulum and iliac wing appear normal.
+Femoral head appears normal and cartilagenous.
+Central ossific nucleus not visualised in femoral head on either side.
+No joint effusion.
+No intramusclar fluid collection.
+Right angle Alpha - 61
+Beta - 56
+Left angle Alpha - 62
+Beta - 55
+No obvious e/o developmental dysplasia of hip.</t>
+        </is>
+      </c>
+      <c r="AW10" t="inlineStr">
+        <is>
+          <t>;
+Normal study. .</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2025-12-28</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Thyroid Test</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
+      <c r="N11" t="inlineStr"/>
+      <c r="O11" t="inlineStr"/>
+      <c r="P11" t="inlineStr"/>
+      <c r="Q11" t="inlineStr"/>
+      <c r="R11" t="inlineStr"/>
+      <c r="S11" t="inlineStr"/>
+      <c r="T11" t="inlineStr"/>
+      <c r="U11" t="inlineStr"/>
+      <c r="V11" t="inlineStr"/>
+      <c r="W11" t="inlineStr"/>
+      <c r="X11" t="inlineStr"/>
+      <c r="Y11" t="inlineStr"/>
+      <c r="Z11" t="inlineStr"/>
+      <c r="AA11" t="inlineStr"/>
+      <c r="AB11" t="inlineStr"/>
+      <c r="AC11" t="inlineStr"/>
+      <c r="AD11" t="n">
+        <v>176.2</v>
+      </c>
+      <c r="AE11" t="n">
+        <v>10.9</v>
+      </c>
+      <c r="AF11" t="n">
+        <v>2.98</v>
+      </c>
+      <c r="AG11" t="inlineStr"/>
+      <c r="AH11" t="inlineStr"/>
+      <c r="AI11" t="inlineStr"/>
+      <c r="AJ11" t="inlineStr"/>
+      <c r="AK11" t="inlineStr"/>
+      <c r="AL11" t="inlineStr"/>
+      <c r="AM11" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="AN11" t="inlineStr"/>
+      <c r="AO11" t="inlineStr"/>
+      <c r="AP11" t="inlineStr"/>
+      <c r="AQ11" t="inlineStr"/>
+      <c r="AR11" t="inlineStr"/>
+      <c r="AS11" t="inlineStr"/>
+      <c r="AT11" t="inlineStr"/>
+      <c r="AU11" t="inlineStr"/>
+      <c r="AV11" t="inlineStr"/>
+      <c r="AW11" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
family member feature added
</commit_message>
<xml_diff>
--- a/data/reports/test_reports.xlsx
+++ b/data/reports/test_reports.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AW11"/>
+  <dimension ref="A1:AW19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1488,10 +1488,8 @@
       <c r="AJ11" t="inlineStr"/>
       <c r="AK11" t="inlineStr"/>
       <c r="AL11" t="inlineStr"/>
-      <c r="AM11" t="inlineStr">
-        <is>
-          <t>90</t>
-        </is>
+      <c r="AM11" t="n">
+        <v>90</v>
       </c>
       <c r="AN11" t="inlineStr"/>
       <c r="AO11" t="inlineStr"/>
@@ -1504,6 +1502,958 @@
       <c r="AV11" t="inlineStr"/>
       <c r="AW11" t="inlineStr"/>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2025-12-28</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Ultrasound Report</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
+      <c r="M12" t="inlineStr"/>
+      <c r="N12" t="inlineStr"/>
+      <c r="O12" t="inlineStr"/>
+      <c r="P12" t="inlineStr"/>
+      <c r="Q12" t="inlineStr"/>
+      <c r="R12" t="inlineStr"/>
+      <c r="S12" t="inlineStr"/>
+      <c r="T12" t="inlineStr"/>
+      <c r="U12" t="inlineStr"/>
+      <c r="V12" t="inlineStr"/>
+      <c r="W12" t="inlineStr"/>
+      <c r="X12" t="inlineStr"/>
+      <c r="Y12" t="inlineStr"/>
+      <c r="Z12" t="inlineStr"/>
+      <c r="AA12" t="inlineStr"/>
+      <c r="AB12" t="inlineStr"/>
+      <c r="AC12" t="inlineStr"/>
+      <c r="AD12" t="inlineStr"/>
+      <c r="AE12" t="inlineStr"/>
+      <c r="AF12" t="inlineStr"/>
+      <c r="AG12" t="inlineStr"/>
+      <c r="AH12" t="inlineStr"/>
+      <c r="AI12" t="inlineStr"/>
+      <c r="AJ12" t="inlineStr"/>
+      <c r="AK12" t="inlineStr"/>
+      <c r="AL12" t="inlineStr">
+        <is>
+          <t>Aagaaz</t>
+        </is>
+      </c>
+      <c r="AM12" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN12" t="inlineStr"/>
+      <c r="AO12" t="n">
+        <v>68</v>
+      </c>
+      <c r="AP12" t="inlineStr"/>
+      <c r="AQ12" t="n">
+        <v>48</v>
+      </c>
+      <c r="AR12" t="inlineStr"/>
+      <c r="AS12" t="inlineStr"/>
+      <c r="AT12" t="inlineStr"/>
+      <c r="AU12" t="inlineStr"/>
+      <c r="AV12" t="inlineStr"/>
+      <c r="AW12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2025-12-28</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Complete Blood Picture (CBP)</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>11.3</v>
+      </c>
+      <c r="D13" t="n">
+        <v>3.78</v>
+      </c>
+      <c r="E13" t="n">
+        <v>10.84</v>
+      </c>
+      <c r="F13" t="n">
+        <v>486</v>
+      </c>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="n">
+        <v>13</v>
+      </c>
+      <c r="J13" t="n">
+        <v>9</v>
+      </c>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr"/>
+      <c r="M13" t="inlineStr"/>
+      <c r="N13" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="O13" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="P13" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>34</v>
+      </c>
+      <c r="R13" t="n">
+        <v>27</v>
+      </c>
+      <c r="S13" t="n">
+        <v>360</v>
+      </c>
+      <c r="T13" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="U13" t="n">
+        <v>46</v>
+      </c>
+      <c r="V13" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="W13" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="X13" t="inlineStr"/>
+      <c r="Y13" t="n">
+        <v>78</v>
+      </c>
+      <c r="Z13" t="n">
+        <v>25.4</v>
+      </c>
+      <c r="AA13" t="n">
+        <v>32.6</v>
+      </c>
+      <c r="AB13" t="n">
+        <v>12.7</v>
+      </c>
+      <c r="AC13" t="n">
+        <v>8.199999999999999</v>
+      </c>
+      <c r="AD13" t="n">
+        <v>3</v>
+      </c>
+      <c r="AE13" t="n">
+        <v>4</v>
+      </c>
+      <c r="AF13" t="n">
+        <v>2.98</v>
+      </c>
+      <c r="AG13" t="n">
+        <v>26</v>
+      </c>
+      <c r="AH13" t="n">
+        <v>70</v>
+      </c>
+      <c r="AI13" t="n">
+        <v>2</v>
+      </c>
+      <c r="AJ13" t="n">
+        <v>2</v>
+      </c>
+      <c r="AK13" t="inlineStr"/>
+      <c r="AL13" t="inlineStr">
+        <is>
+          <t>KASHV</t>
+        </is>
+      </c>
+      <c r="AM13" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN13" t="inlineStr"/>
+      <c r="AO13" t="inlineStr"/>
+      <c r="AP13" t="inlineStr"/>
+      <c r="AQ13" t="inlineStr"/>
+      <c r="AR13" t="inlineStr"/>
+      <c r="AS13" t="inlineStr"/>
+      <c r="AT13" t="inlineStr"/>
+      <c r="AU13" t="inlineStr"/>
+      <c r="AV13" t="inlineStr"/>
+      <c r="AW13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2025-12-28</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Complete Blood Picture (CBP)</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>11.3</v>
+      </c>
+      <c r="D14" t="n">
+        <v>3.78</v>
+      </c>
+      <c r="E14" t="n">
+        <v>10.84</v>
+      </c>
+      <c r="F14" t="n">
+        <v>486</v>
+      </c>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="n">
+        <v>13</v>
+      </c>
+      <c r="J14" t="n">
+        <v>9</v>
+      </c>
+      <c r="K14" t="inlineStr"/>
+      <c r="L14" t="inlineStr"/>
+      <c r="M14" t="inlineStr"/>
+      <c r="N14" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="O14" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="P14" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>34</v>
+      </c>
+      <c r="R14" t="n">
+        <v>27</v>
+      </c>
+      <c r="S14" t="n">
+        <v>360</v>
+      </c>
+      <c r="T14" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="U14" t="n">
+        <v>46</v>
+      </c>
+      <c r="V14" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="W14" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="X14" t="inlineStr"/>
+      <c r="Y14" t="n">
+        <v>78</v>
+      </c>
+      <c r="Z14" t="n">
+        <v>25.4</v>
+      </c>
+      <c r="AA14" t="n">
+        <v>32.6</v>
+      </c>
+      <c r="AB14" t="n">
+        <v>12.7</v>
+      </c>
+      <c r="AC14" t="n">
+        <v>8.199999999999999</v>
+      </c>
+      <c r="AD14" t="n">
+        <v>3</v>
+      </c>
+      <c r="AE14" t="n">
+        <v>4</v>
+      </c>
+      <c r="AF14" t="n">
+        <v>2.98</v>
+      </c>
+      <c r="AG14" t="n">
+        <v>26</v>
+      </c>
+      <c r="AH14" t="n">
+        <v>70</v>
+      </c>
+      <c r="AI14" t="n">
+        <v>2</v>
+      </c>
+      <c r="AJ14" t="n">
+        <v>2</v>
+      </c>
+      <c r="AK14" t="inlineStr"/>
+      <c r="AL14" t="inlineStr">
+        <is>
+          <t>KASHV</t>
+        </is>
+      </c>
+      <c r="AM14" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN14" t="inlineStr"/>
+      <c r="AO14" t="inlineStr"/>
+      <c r="AP14" t="inlineStr"/>
+      <c r="AQ14" t="inlineStr"/>
+      <c r="AR14" t="inlineStr"/>
+      <c r="AS14" t="inlineStr"/>
+      <c r="AT14" t="inlineStr"/>
+      <c r="AU14" t="inlineStr"/>
+      <c r="AV14" t="inlineStr"/>
+      <c r="AW14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2025-12-28</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Complete Blood Picture (CBP)</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>11.3</v>
+      </c>
+      <c r="D15" t="n">
+        <v>3.78</v>
+      </c>
+      <c r="E15" t="n">
+        <v>10.84</v>
+      </c>
+      <c r="F15" t="n">
+        <v>486</v>
+      </c>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr"/>
+      <c r="I15" t="n">
+        <v>13</v>
+      </c>
+      <c r="J15" t="n">
+        <v>9</v>
+      </c>
+      <c r="K15" t="inlineStr"/>
+      <c r="L15" t="inlineStr"/>
+      <c r="M15" t="inlineStr"/>
+      <c r="N15" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="O15" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="P15" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>34</v>
+      </c>
+      <c r="R15" t="n">
+        <v>27</v>
+      </c>
+      <c r="S15" t="n">
+        <v>360</v>
+      </c>
+      <c r="T15" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="U15" t="n">
+        <v>46</v>
+      </c>
+      <c r="V15" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="W15" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="X15" t="inlineStr"/>
+      <c r="Y15" t="n">
+        <v>78</v>
+      </c>
+      <c r="Z15" t="n">
+        <v>25.4</v>
+      </c>
+      <c r="AA15" t="n">
+        <v>32.6</v>
+      </c>
+      <c r="AB15" t="n">
+        <v>12.7</v>
+      </c>
+      <c r="AC15" t="n">
+        <v>8.199999999999999</v>
+      </c>
+      <c r="AD15" t="n">
+        <v>3</v>
+      </c>
+      <c r="AE15" t="n">
+        <v>4</v>
+      </c>
+      <c r="AF15" t="n">
+        <v>2.98</v>
+      </c>
+      <c r="AG15" t="n">
+        <v>26</v>
+      </c>
+      <c r="AH15" t="n">
+        <v>70</v>
+      </c>
+      <c r="AI15" t="n">
+        <v>2</v>
+      </c>
+      <c r="AJ15" t="n">
+        <v>2</v>
+      </c>
+      <c r="AK15" t="inlineStr"/>
+      <c r="AL15" t="inlineStr">
+        <is>
+          <t>KASHV</t>
+        </is>
+      </c>
+      <c r="AM15" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN15" t="inlineStr"/>
+      <c r="AO15" t="inlineStr"/>
+      <c r="AP15" t="inlineStr"/>
+      <c r="AQ15" t="inlineStr"/>
+      <c r="AR15" t="inlineStr"/>
+      <c r="AS15" t="inlineStr"/>
+      <c r="AT15" t="inlineStr"/>
+      <c r="AU15" t="inlineStr"/>
+      <c r="AV15" t="inlineStr"/>
+      <c r="AW15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2025-12-28</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Complete Blood Picture (CBP)</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>11.3</v>
+      </c>
+      <c r="D16" t="n">
+        <v>3.78</v>
+      </c>
+      <c r="E16" t="n">
+        <v>10.84</v>
+      </c>
+      <c r="F16" t="n">
+        <v>486</v>
+      </c>
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr"/>
+      <c r="I16" t="n">
+        <v>13</v>
+      </c>
+      <c r="J16" t="n">
+        <v>9</v>
+      </c>
+      <c r="K16" t="inlineStr"/>
+      <c r="L16" t="inlineStr"/>
+      <c r="M16" t="inlineStr"/>
+      <c r="N16" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="O16" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="P16" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>34</v>
+      </c>
+      <c r="R16" t="n">
+        <v>27</v>
+      </c>
+      <c r="S16" t="n">
+        <v>360</v>
+      </c>
+      <c r="T16" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="U16" t="n">
+        <v>46</v>
+      </c>
+      <c r="V16" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="W16" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="X16" t="inlineStr"/>
+      <c r="Y16" t="n">
+        <v>78</v>
+      </c>
+      <c r="Z16" t="n">
+        <v>25.4</v>
+      </c>
+      <c r="AA16" t="n">
+        <v>32.6</v>
+      </c>
+      <c r="AB16" t="n">
+        <v>12.7</v>
+      </c>
+      <c r="AC16" t="n">
+        <v>8.199999999999999</v>
+      </c>
+      <c r="AD16" t="n">
+        <v>3</v>
+      </c>
+      <c r="AE16" t="n">
+        <v>4</v>
+      </c>
+      <c r="AF16" t="n">
+        <v>2.98</v>
+      </c>
+      <c r="AG16" t="n">
+        <v>26</v>
+      </c>
+      <c r="AH16" t="n">
+        <v>70</v>
+      </c>
+      <c r="AI16" t="n">
+        <v>2</v>
+      </c>
+      <c r="AJ16" t="n">
+        <v>2</v>
+      </c>
+      <c r="AK16" t="inlineStr"/>
+      <c r="AL16" t="inlineStr">
+        <is>
+          <t>KASHV</t>
+        </is>
+      </c>
+      <c r="AM16" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN16" t="inlineStr"/>
+      <c r="AO16" t="inlineStr"/>
+      <c r="AP16" t="inlineStr"/>
+      <c r="AQ16" t="inlineStr"/>
+      <c r="AR16" t="inlineStr"/>
+      <c r="AS16" t="inlineStr"/>
+      <c r="AT16" t="inlineStr"/>
+      <c r="AU16" t="inlineStr"/>
+      <c r="AV16" t="inlineStr"/>
+      <c r="AW16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2025-12-29</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Ultrasound Report</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>11.3</v>
+      </c>
+      <c r="D17" t="n">
+        <v>3.78</v>
+      </c>
+      <c r="E17" t="n">
+        <v>10.84</v>
+      </c>
+      <c r="F17" t="n">
+        <v>486</v>
+      </c>
+      <c r="G17" t="inlineStr"/>
+      <c r="H17" t="inlineStr"/>
+      <c r="I17" t="n">
+        <v>13</v>
+      </c>
+      <c r="J17" t="n">
+        <v>9</v>
+      </c>
+      <c r="K17" t="inlineStr"/>
+      <c r="L17" t="inlineStr"/>
+      <c r="M17" t="inlineStr"/>
+      <c r="N17" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="O17" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="P17" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>34</v>
+      </c>
+      <c r="R17" t="n">
+        <v>27</v>
+      </c>
+      <c r="S17" t="n">
+        <v>360</v>
+      </c>
+      <c r="T17" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="U17" t="n">
+        <v>46</v>
+      </c>
+      <c r="V17" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="W17" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="X17" t="inlineStr"/>
+      <c r="Y17" t="n">
+        <v>78</v>
+      </c>
+      <c r="Z17" t="n">
+        <v>25.4</v>
+      </c>
+      <c r="AA17" t="n">
+        <v>32.6</v>
+      </c>
+      <c r="AB17" t="n">
+        <v>12.7</v>
+      </c>
+      <c r="AC17" t="n">
+        <v>8.199999999999999</v>
+      </c>
+      <c r="AD17" t="n">
+        <v>3</v>
+      </c>
+      <c r="AE17" t="n">
+        <v>4</v>
+      </c>
+      <c r="AF17" t="n">
+        <v>2.98</v>
+      </c>
+      <c r="AG17" t="n">
+        <v>26</v>
+      </c>
+      <c r="AH17" t="n">
+        <v>70</v>
+      </c>
+      <c r="AI17" t="n">
+        <v>2</v>
+      </c>
+      <c r="AJ17" t="n">
+        <v>2</v>
+      </c>
+      <c r="AK17" t="inlineStr"/>
+      <c r="AL17" t="inlineStr">
+        <is>
+          <t>KASHV</t>
+        </is>
+      </c>
+      <c r="AM17" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN17" t="inlineStr"/>
+      <c r="AO17" t="n">
+        <v>68</v>
+      </c>
+      <c r="AP17" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="AQ17" t="n">
+        <v>48</v>
+      </c>
+      <c r="AR17" t="inlineStr"/>
+      <c r="AS17" t="inlineStr">
+        <is>
+          <t>43 x 19 mm</t>
+        </is>
+      </c>
+      <c r="AT17" t="inlineStr">
+        <is>
+          <t>48 x 22 mm</t>
+        </is>
+      </c>
+      <c r="AU17" t="inlineStr"/>
+      <c r="AV17" t="inlineStr">
+        <is>
+          <t>Acetabulum and iliac wing appear normal.
+Femoral head appears normal and cartilagenous.
+Central ossific nucleus not visualised in femoral head on either side.
+No joint effusion.
+No intramusclar fluid collection.
+Right angle Alpha - 61
+Beta - 56
+Left angle Alpha - 62
+Beta - 55
+No obvious e/o developmental dysplasia of hip.</t>
+        </is>
+      </c>
+      <c r="AW17" t="inlineStr">
+        <is>
+          <t>;
+Normal study. .</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2025-12-29</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Liver Function Test (LFT)</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>11.3</v>
+      </c>
+      <c r="D18" t="n">
+        <v>3.78</v>
+      </c>
+      <c r="E18" t="n">
+        <v>10.84</v>
+      </c>
+      <c r="F18" t="n">
+        <v>486</v>
+      </c>
+      <c r="G18" t="inlineStr"/>
+      <c r="H18" t="inlineStr"/>
+      <c r="I18" t="n">
+        <v>13</v>
+      </c>
+      <c r="J18" t="n">
+        <v>9</v>
+      </c>
+      <c r="K18" t="inlineStr"/>
+      <c r="L18" t="inlineStr"/>
+      <c r="M18" t="inlineStr"/>
+      <c r="N18" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="O18" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="P18" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>34</v>
+      </c>
+      <c r="R18" t="n">
+        <v>27</v>
+      </c>
+      <c r="S18" t="n">
+        <v>360</v>
+      </c>
+      <c r="T18" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="U18" t="n">
+        <v>46</v>
+      </c>
+      <c r="V18" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="W18" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="X18" t="inlineStr"/>
+      <c r="Y18" t="n">
+        <v>78</v>
+      </c>
+      <c r="Z18" t="n">
+        <v>25.4</v>
+      </c>
+      <c r="AA18" t="n">
+        <v>32.6</v>
+      </c>
+      <c r="AB18" t="n">
+        <v>12.7</v>
+      </c>
+      <c r="AC18" t="n">
+        <v>8.199999999999999</v>
+      </c>
+      <c r="AD18" t="n">
+        <v>3</v>
+      </c>
+      <c r="AE18" t="n">
+        <v>4</v>
+      </c>
+      <c r="AF18" t="n">
+        <v>2.98</v>
+      </c>
+      <c r="AG18" t="n">
+        <v>26</v>
+      </c>
+      <c r="AH18" t="n">
+        <v>70</v>
+      </c>
+      <c r="AI18" t="n">
+        <v>2</v>
+      </c>
+      <c r="AJ18" t="n">
+        <v>2</v>
+      </c>
+      <c r="AK18" t="inlineStr"/>
+      <c r="AL18" t="inlineStr">
+        <is>
+          <t>KASHV</t>
+        </is>
+      </c>
+      <c r="AM18" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN18" t="inlineStr"/>
+      <c r="AO18" t="inlineStr"/>
+      <c r="AP18" t="inlineStr"/>
+      <c r="AQ18" t="inlineStr"/>
+      <c r="AR18" t="inlineStr"/>
+      <c r="AS18" t="inlineStr"/>
+      <c r="AT18" t="inlineStr"/>
+      <c r="AU18" t="inlineStr"/>
+      <c r="AV18" t="inlineStr"/>
+      <c r="AW18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2025-12-29</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Complete Blood Picture (CBP)</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>11.3</v>
+      </c>
+      <c r="D19" t="n">
+        <v>3.78</v>
+      </c>
+      <c r="E19" t="n">
+        <v>10.84</v>
+      </c>
+      <c r="F19" t="n">
+        <v>486</v>
+      </c>
+      <c r="G19" t="inlineStr"/>
+      <c r="H19" t="inlineStr"/>
+      <c r="I19" t="n">
+        <v>13</v>
+      </c>
+      <c r="J19" t="n">
+        <v>9</v>
+      </c>
+      <c r="K19" t="inlineStr"/>
+      <c r="L19" t="inlineStr"/>
+      <c r="M19" t="inlineStr"/>
+      <c r="N19" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="O19" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="P19" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>34</v>
+      </c>
+      <c r="R19" t="n">
+        <v>27</v>
+      </c>
+      <c r="S19" t="n">
+        <v>360</v>
+      </c>
+      <c r="T19" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="U19" t="n">
+        <v>46</v>
+      </c>
+      <c r="V19" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="W19" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="X19" t="inlineStr"/>
+      <c r="Y19" t="n">
+        <v>78</v>
+      </c>
+      <c r="Z19" t="n">
+        <v>25.4</v>
+      </c>
+      <c r="AA19" t="n">
+        <v>32.6</v>
+      </c>
+      <c r="AB19" t="n">
+        <v>12.7</v>
+      </c>
+      <c r="AC19" t="n">
+        <v>8.199999999999999</v>
+      </c>
+      <c r="AD19" t="n">
+        <v>3</v>
+      </c>
+      <c r="AE19" t="n">
+        <v>4</v>
+      </c>
+      <c r="AF19" t="n">
+        <v>2.98</v>
+      </c>
+      <c r="AG19" t="n">
+        <v>26</v>
+      </c>
+      <c r="AH19" t="n">
+        <v>70</v>
+      </c>
+      <c r="AI19" t="n">
+        <v>2</v>
+      </c>
+      <c r="AJ19" t="n">
+        <v>2</v>
+      </c>
+      <c r="AK19" t="inlineStr"/>
+      <c r="AL19" t="inlineStr">
+        <is>
+          <t>KASHV</t>
+        </is>
+      </c>
+      <c r="AM19" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AN19" t="inlineStr"/>
+      <c r="AO19" t="inlineStr"/>
+      <c r="AP19" t="inlineStr"/>
+      <c r="AQ19" t="inlineStr"/>
+      <c r="AR19" t="inlineStr"/>
+      <c r="AS19" t="inlineStr"/>
+      <c r="AT19" t="inlineStr"/>
+      <c r="AU19" t="inlineStr"/>
+      <c r="AV19" t="inlineStr"/>
+      <c r="AW19" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Improved trend graph feature
</commit_message>
<xml_diff>
--- a/data/reports/test_reports.xlsx
+++ b/data/reports/test_reports.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -16,7 +16,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -55,11 +58,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AW19"/>
+  <dimension ref="A1:AW23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -681,20 +685,22 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>2025-12-19</t>
-        </is>
+      <c r="A2" s="2" t="n">
+        <v>45908</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
           <t>Liver Function Test (LFT)</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr"/>
+      <c r="C2" t="n">
+        <v>11.3</v>
+      </c>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
+      <c r="F2" t="n">
+        <v>416</v>
+      </c>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="n">
@@ -706,37 +712,79 @@
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr"/>
-      <c r="N2" t="inlineStr"/>
+      <c r="N2" t="n">
+        <v>0.4</v>
+      </c>
       <c r="O2" t="n">
         <v>0.2</v>
       </c>
       <c r="P2" t="n">
         <v>0.2</v>
       </c>
-      <c r="Q2" t="inlineStr"/>
-      <c r="R2" t="inlineStr"/>
+      <c r="Q2" t="n">
+        <v>34</v>
+      </c>
+      <c r="R2" t="n">
+        <v>27</v>
+      </c>
       <c r="S2" t="inlineStr"/>
-      <c r="T2" t="inlineStr"/>
-      <c r="U2" t="inlineStr"/>
-      <c r="V2" t="inlineStr"/>
-      <c r="W2" t="inlineStr"/>
+      <c r="T2" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="U2" t="n">
+        <v>46</v>
+      </c>
+      <c r="V2" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="W2" t="n">
+        <v>2.4</v>
+      </c>
       <c r="X2" t="inlineStr"/>
-      <c r="Y2" t="inlineStr"/>
-      <c r="Z2" t="inlineStr"/>
-      <c r="AA2" t="inlineStr"/>
-      <c r="AB2" t="inlineStr"/>
-      <c r="AC2" t="inlineStr"/>
+      <c r="Y2" t="n">
+        <v>78</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>25.4</v>
+      </c>
+      <c r="AA2" t="n">
+        <v>32.6</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>12.7</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>8.199999999999999</v>
+      </c>
       <c r="AD2" t="inlineStr"/>
       <c r="AE2" t="inlineStr"/>
       <c r="AF2" t="inlineStr"/>
-      <c r="AG2" t="inlineStr"/>
-      <c r="AH2" t="inlineStr"/>
-      <c r="AI2" t="inlineStr"/>
-      <c r="AJ2" t="inlineStr"/>
+      <c r="AG2" t="n">
+        <v>26</v>
+      </c>
+      <c r="AH2" t="n">
+        <v>70</v>
+      </c>
+      <c r="AI2" t="n">
+        <v>2</v>
+      </c>
+      <c r="AJ2" t="n">
+        <v>2</v>
+      </c>
       <c r="AK2" t="inlineStr"/>
-      <c r="AL2" t="inlineStr"/>
-      <c r="AM2" t="inlineStr"/>
-      <c r="AN2" t="inlineStr"/>
+      <c r="AL2" t="inlineStr">
+        <is>
+          <t>KASHV</t>
+        </is>
+      </c>
+      <c r="AM2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN2" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
       <c r="AO2" t="inlineStr"/>
       <c r="AP2" t="inlineStr"/>
       <c r="AQ2" t="inlineStr"/>
@@ -748,14 +796,12 @@
       <c r="AW2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2025-12-19</t>
-        </is>
+      <c r="A3" s="2" t="n">
+        <v>46010</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Thyroid Test</t>
+          <t>Liver Function Test (LFT)</t>
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
@@ -815,14 +861,12 @@
       <c r="AW3" t="inlineStr"/>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>2025-12-19</t>
-        </is>
+      <c r="A4" s="2" t="n">
+        <v>46010</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Complete Blood Picture (CBP)</t>
+          <t>Comprehensive Health Check</t>
         </is>
       </c>
       <c r="C4" t="inlineStr"/>
@@ -882,14 +926,12 @@
       <c r="AW4" t="inlineStr"/>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>2025-12-19</t>
-        </is>
+      <c r="A5" s="2" t="n">
+        <v>46010</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Comprehensive Health Check</t>
+          <t>Liver Function Test (LFT)</t>
         </is>
       </c>
       <c r="C5" t="inlineStr"/>
@@ -949,14 +991,12 @@
       <c r="AW5" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>2025-12-19</t>
-        </is>
+      <c r="A6" s="2" t="n">
+        <v>46010</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Liver Function Test (LFT)</t>
+          <t>Thyroid Test</t>
         </is>
       </c>
       <c r="C6" t="inlineStr"/>
@@ -1016,28 +1056,18 @@
       <c r="AW6" t="inlineStr"/>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>2025-12-21</t>
-        </is>
+      <c r="A7" s="2" t="n">
+        <v>46010</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
           <t>Complete Blood Picture (CBP)</t>
         </is>
       </c>
-      <c r="C7" t="n">
-        <v>11.3</v>
-      </c>
-      <c r="D7" t="n">
-        <v>4.45</v>
-      </c>
-      <c r="E7" t="n">
-        <v>10.54</v>
-      </c>
-      <c r="F7" t="n">
-        <v>416</v>
-      </c>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
       <c r="I7" t="n">
@@ -1049,70 +1079,34 @@
       <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr"/>
       <c r="M7" t="inlineStr"/>
-      <c r="N7" t="n">
-        <v>0.4</v>
-      </c>
+      <c r="N7" t="inlineStr"/>
       <c r="O7" t="n">
         <v>0.2</v>
       </c>
       <c r="P7" t="n">
         <v>0.2</v>
       </c>
-      <c r="Q7" t="n">
-        <v>34</v>
-      </c>
-      <c r="R7" t="n">
-        <v>5</v>
-      </c>
-      <c r="S7" t="n">
-        <v>219</v>
-      </c>
+      <c r="Q7" t="inlineStr"/>
+      <c r="R7" t="inlineStr"/>
+      <c r="S7" t="inlineStr"/>
       <c r="T7" t="inlineStr"/>
-      <c r="U7" t="n">
-        <v>4.6</v>
-      </c>
-      <c r="V7" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="W7" t="n">
-        <v>2.4</v>
-      </c>
-      <c r="X7" t="n">
-        <v>34.7</v>
-      </c>
-      <c r="Y7" t="n">
-        <v>78</v>
-      </c>
-      <c r="Z7" t="n">
-        <v>25.4</v>
-      </c>
-      <c r="AA7" t="n">
-        <v>32</v>
-      </c>
-      <c r="AB7" t="n">
-        <v>12</v>
-      </c>
-      <c r="AC7" t="n">
-        <v>8.199999999999999</v>
-      </c>
+      <c r="U7" t="inlineStr"/>
+      <c r="V7" t="inlineStr"/>
+      <c r="W7" t="inlineStr"/>
+      <c r="X7" t="inlineStr"/>
+      <c r="Y7" t="inlineStr"/>
+      <c r="Z7" t="inlineStr"/>
+      <c r="AA7" t="inlineStr"/>
+      <c r="AB7" t="inlineStr"/>
+      <c r="AC7" t="inlineStr"/>
       <c r="AD7" t="inlineStr"/>
       <c r="AE7" t="inlineStr"/>
       <c r="AF7" t="inlineStr"/>
-      <c r="AG7" t="n">
-        <v>26</v>
-      </c>
-      <c r="AH7" t="n">
-        <v>79</v>
-      </c>
-      <c r="AI7" t="n">
-        <v>2</v>
-      </c>
-      <c r="AJ7" t="n">
-        <v>2</v>
-      </c>
-      <c r="AK7" t="n">
-        <v>10</v>
-      </c>
+      <c r="AG7" t="inlineStr"/>
+      <c r="AH7" t="inlineStr"/>
+      <c r="AI7" t="inlineStr"/>
+      <c r="AJ7" t="inlineStr"/>
+      <c r="AK7" t="inlineStr"/>
       <c r="AL7" t="inlineStr"/>
       <c r="AM7" t="inlineStr"/>
       <c r="AN7" t="inlineStr"/>
@@ -1127,14 +1121,12 @@
       <c r="AW7" t="inlineStr"/>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>2025-12-27</t>
-        </is>
+      <c r="A8" s="2" t="n">
+        <v>46012</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Liver Function Test (LFT)</t>
+          <t>Complete Blood Picture (CBP)</t>
         </is>
       </c>
       <c r="C8" t="n">
@@ -1238,212 +1230,240 @@
       <c r="AW8" t="inlineStr"/>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>2025-12-28</t>
-        </is>
+      <c r="A9" s="2" t="n">
+        <v>46018</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Vitals Check</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr"/>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
+          <t>Liver Function Test (LFT)</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>11.3</v>
+      </c>
+      <c r="D9" t="n">
+        <v>4.45</v>
+      </c>
+      <c r="E9" t="n">
+        <v>10.54</v>
+      </c>
+      <c r="F9" t="n">
+        <v>416</v>
+      </c>
       <c r="G9" t="inlineStr"/>
       <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
+      <c r="I9" t="n">
+        <v>13</v>
+      </c>
+      <c r="J9" t="n">
+        <v>9</v>
+      </c>
       <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr"/>
       <c r="M9" t="inlineStr"/>
-      <c r="N9" t="inlineStr"/>
-      <c r="O9" t="inlineStr"/>
-      <c r="P9" t="inlineStr"/>
-      <c r="Q9" t="inlineStr"/>
-      <c r="R9" t="inlineStr"/>
-      <c r="S9" t="inlineStr"/>
+      <c r="N9" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="O9" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="P9" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>34</v>
+      </c>
+      <c r="R9" t="n">
+        <v>5</v>
+      </c>
+      <c r="S9" t="n">
+        <v>219</v>
+      </c>
       <c r="T9" t="inlineStr"/>
-      <c r="U9" t="inlineStr"/>
-      <c r="V9" t="inlineStr"/>
-      <c r="W9" t="inlineStr"/>
-      <c r="X9" t="inlineStr"/>
-      <c r="Y9" t="inlineStr"/>
-      <c r="Z9" t="inlineStr"/>
-      <c r="AA9" t="inlineStr"/>
-      <c r="AB9" t="inlineStr"/>
-      <c r="AC9" t="inlineStr"/>
+      <c r="U9" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="V9" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="W9" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="X9" t="n">
+        <v>34.7</v>
+      </c>
+      <c r="Y9" t="n">
+        <v>78</v>
+      </c>
+      <c r="Z9" t="n">
+        <v>25.4</v>
+      </c>
+      <c r="AA9" t="n">
+        <v>32</v>
+      </c>
+      <c r="AB9" t="n">
+        <v>12</v>
+      </c>
+      <c r="AC9" t="n">
+        <v>8.199999999999999</v>
+      </c>
       <c r="AD9" t="inlineStr"/>
       <c r="AE9" t="inlineStr"/>
       <c r="AF9" t="inlineStr"/>
-      <c r="AG9" t="inlineStr"/>
-      <c r="AH9" t="inlineStr"/>
-      <c r="AI9" t="inlineStr"/>
-      <c r="AJ9" t="inlineStr"/>
-      <c r="AK9" t="inlineStr"/>
+      <c r="AG9" t="n">
+        <v>26</v>
+      </c>
+      <c r="AH9" t="n">
+        <v>79</v>
+      </c>
+      <c r="AI9" t="n">
+        <v>2</v>
+      </c>
+      <c r="AJ9" t="n">
+        <v>2</v>
+      </c>
+      <c r="AK9" t="n">
+        <v>10</v>
+      </c>
       <c r="AL9" t="inlineStr"/>
-      <c r="AM9" t="n">
-        <v>1</v>
-      </c>
-      <c r="AN9" t="inlineStr">
-        <is>
-          <t>Gender Leger</t>
-        </is>
-      </c>
-      <c r="AO9" t="n">
-        <v>68</v>
-      </c>
-      <c r="AP9" t="inlineStr">
-        <is>
-          <t>Normal</t>
-        </is>
-      </c>
-      <c r="AQ9" t="n">
-        <v>48</v>
-      </c>
+      <c r="AM9" t="inlineStr"/>
+      <c r="AN9" t="inlineStr"/>
+      <c r="AO9" t="inlineStr"/>
+      <c r="AP9" t="inlineStr"/>
+      <c r="AQ9" t="inlineStr"/>
       <c r="AR9" t="inlineStr"/>
-      <c r="AS9" t="inlineStr">
-        <is>
-          <t>43 x 19 mm</t>
-        </is>
-      </c>
-      <c r="AT9" t="inlineStr">
-        <is>
-          <t>48 x 22 mm</t>
-        </is>
-      </c>
+      <c r="AS9" t="inlineStr"/>
+      <c r="AT9" t="inlineStr"/>
       <c r="AU9" t="inlineStr"/>
-      <c r="AV9" t="inlineStr">
-        <is>
-          <t>Acetabulum and iliac wing appear normal.
-Femoral head appears normal and cartilagenous.
-Central ossific nucleus not visualised in femoral head on either side.
-No joint effusion.
-No intramusclar fluid collection.
-Right angle Alpha - 61
-Beta - 56
-Left angle Alpha - 62
-Beta - 55
-No obvious e/o developmental dysplasia of hip.</t>
-        </is>
-      </c>
-      <c r="AW9" t="inlineStr">
-        <is>
-          <t>;
-Normal study. .</t>
-        </is>
-      </c>
+      <c r="AV9" t="inlineStr"/>
+      <c r="AW9" t="inlineStr"/>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>2025-12-28</t>
-        </is>
+      <c r="A10" s="2" t="n">
+        <v>46019</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Ultrasound Report</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
+          <t>Complete Blood Picture (CBP)</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>11.3</v>
+      </c>
+      <c r="D10" t="n">
+        <v>3.78</v>
+      </c>
+      <c r="E10" t="n">
+        <v>10.84</v>
+      </c>
+      <c r="F10" t="n">
+        <v>486</v>
+      </c>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
+      <c r="I10" t="n">
+        <v>13</v>
+      </c>
+      <c r="J10" t="n">
+        <v>9</v>
+      </c>
       <c r="K10" t="inlineStr"/>
       <c r="L10" t="inlineStr"/>
       <c r="M10" t="inlineStr"/>
-      <c r="N10" t="inlineStr"/>
-      <c r="O10" t="inlineStr"/>
-      <c r="P10" t="inlineStr"/>
-      <c r="Q10" t="inlineStr"/>
-      <c r="R10" t="inlineStr"/>
-      <c r="S10" t="inlineStr"/>
-      <c r="T10" t="inlineStr"/>
-      <c r="U10" t="inlineStr"/>
-      <c r="V10" t="inlineStr"/>
-      <c r="W10" t="inlineStr"/>
+      <c r="N10" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="O10" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="P10" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>34</v>
+      </c>
+      <c r="R10" t="n">
+        <v>27</v>
+      </c>
+      <c r="S10" t="n">
+        <v>360</v>
+      </c>
+      <c r="T10" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="U10" t="n">
+        <v>46</v>
+      </c>
+      <c r="V10" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="W10" t="n">
+        <v>2.4</v>
+      </c>
       <c r="X10" t="inlineStr"/>
-      <c r="Y10" t="inlineStr"/>
-      <c r="Z10" t="inlineStr"/>
-      <c r="AA10" t="inlineStr"/>
-      <c r="AB10" t="inlineStr"/>
-      <c r="AC10" t="inlineStr"/>
-      <c r="AD10" t="inlineStr"/>
-      <c r="AE10" t="inlineStr"/>
-      <c r="AF10" t="inlineStr"/>
-      <c r="AG10" t="inlineStr"/>
-      <c r="AH10" t="inlineStr"/>
-      <c r="AI10" t="inlineStr"/>
-      <c r="AJ10" t="inlineStr"/>
+      <c r="Y10" t="n">
+        <v>78</v>
+      </c>
+      <c r="Z10" t="n">
+        <v>25.4</v>
+      </c>
+      <c r="AA10" t="n">
+        <v>32.6</v>
+      </c>
+      <c r="AB10" t="n">
+        <v>12.7</v>
+      </c>
+      <c r="AC10" t="n">
+        <v>8.199999999999999</v>
+      </c>
+      <c r="AD10" t="n">
+        <v>3</v>
+      </c>
+      <c r="AE10" t="n">
+        <v>4</v>
+      </c>
+      <c r="AF10" t="n">
+        <v>2.98</v>
+      </c>
+      <c r="AG10" t="n">
+        <v>26</v>
+      </c>
+      <c r="AH10" t="n">
+        <v>70</v>
+      </c>
+      <c r="AI10" t="n">
+        <v>2</v>
+      </c>
+      <c r="AJ10" t="n">
+        <v>2</v>
+      </c>
       <c r="AK10" t="inlineStr"/>
-      <c r="AL10" t="inlineStr"/>
+      <c r="AL10" t="inlineStr">
+        <is>
+          <t>KASHV</t>
+        </is>
+      </c>
       <c r="AM10" t="n">
         <v>1</v>
       </c>
-      <c r="AN10" t="inlineStr">
-        <is>
-          <t>Gender Leger</t>
-        </is>
-      </c>
-      <c r="AO10" t="n">
-        <v>68</v>
-      </c>
-      <c r="AP10" t="inlineStr">
-        <is>
-          <t>Normal</t>
-        </is>
-      </c>
-      <c r="AQ10" t="n">
-        <v>48</v>
-      </c>
+      <c r="AN10" t="inlineStr"/>
+      <c r="AO10" t="inlineStr"/>
+      <c r="AP10" t="inlineStr"/>
+      <c r="AQ10" t="inlineStr"/>
       <c r="AR10" t="inlineStr"/>
-      <c r="AS10" t="inlineStr">
-        <is>
-          <t>43 x 19 mm</t>
-        </is>
-      </c>
-      <c r="AT10" t="inlineStr">
-        <is>
-          <t>48 x 22 mm</t>
-        </is>
-      </c>
+      <c r="AS10" t="inlineStr"/>
+      <c r="AT10" t="inlineStr"/>
       <c r="AU10" t="inlineStr"/>
-      <c r="AV10" t="inlineStr">
-        <is>
-          <t>Acetabulum and iliac wing appear normal.
-Femoral head appears normal and cartilagenous.
-Central ossific nucleus not visualised in femoral head on either side.
-No joint effusion.
-No intramusclar fluid collection.
-Right angle Alpha - 61
-Beta - 56
-Left angle Alpha - 62
-Beta - 55
-No obvious e/o developmental dysplasia of hip.</t>
-        </is>
-      </c>
-      <c r="AW10" t="inlineStr">
-        <is>
-          <t>;
-Normal study. .</t>
-        </is>
-      </c>
+      <c r="AV10" t="inlineStr"/>
+      <c r="AW10" t="inlineStr"/>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>2025-12-28</t>
-        </is>
+      <c r="A11" s="2" t="n">
+        <v>46019</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Thyroid Test</t>
+          <t>Vitals Check</t>
         </is>
       </c>
       <c r="C11" t="inlineStr"/>
@@ -1473,15 +1493,9 @@
       <c r="AA11" t="inlineStr"/>
       <c r="AB11" t="inlineStr"/>
       <c r="AC11" t="inlineStr"/>
-      <c r="AD11" t="n">
-        <v>176.2</v>
-      </c>
-      <c r="AE11" t="n">
-        <v>10.9</v>
-      </c>
-      <c r="AF11" t="n">
-        <v>2.98</v>
-      </c>
+      <c r="AD11" t="inlineStr"/>
+      <c r="AE11" t="inlineStr"/>
+      <c r="AF11" t="inlineStr"/>
       <c r="AG11" t="inlineStr"/>
       <c r="AH11" t="inlineStr"/>
       <c r="AI11" t="inlineStr"/>
@@ -1489,24 +1503,60 @@
       <c r="AK11" t="inlineStr"/>
       <c r="AL11" t="inlineStr"/>
       <c r="AM11" t="n">
-        <v>90</v>
-      </c>
-      <c r="AN11" t="inlineStr"/>
-      <c r="AO11" t="inlineStr"/>
-      <c r="AP11" t="inlineStr"/>
-      <c r="AQ11" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="AN11" t="inlineStr">
+        <is>
+          <t>Gender Leger</t>
+        </is>
+      </c>
+      <c r="AO11" t="n">
+        <v>68</v>
+      </c>
+      <c r="AP11" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="AQ11" t="n">
+        <v>48</v>
+      </c>
       <c r="AR11" t="inlineStr"/>
-      <c r="AS11" t="inlineStr"/>
-      <c r="AT11" t="inlineStr"/>
+      <c r="AS11" t="inlineStr">
+        <is>
+          <t>43 x 19 mm</t>
+        </is>
+      </c>
+      <c r="AT11" t="inlineStr">
+        <is>
+          <t>48 x 22 mm</t>
+        </is>
+      </c>
       <c r="AU11" t="inlineStr"/>
-      <c r="AV11" t="inlineStr"/>
-      <c r="AW11" t="inlineStr"/>
+      <c r="AV11" t="inlineStr">
+        <is>
+          <t>Acetabulum and iliac wing appear normal.
+Femoral head appears normal and cartilagenous.
+Central ossific nucleus not visualised in femoral head on either side.
+No joint effusion.
+No intramusclar fluid collection.
+Right angle Alpha - 61
+Beta - 56
+Left angle Alpha - 62
+Beta - 55
+No obvious e/o developmental dysplasia of hip.</t>
+        </is>
+      </c>
+      <c r="AW11" t="inlineStr">
+        <is>
+          <t>;
+Normal study. .</t>
+        </is>
+      </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>2025-12-28</t>
-        </is>
+      <c r="A12" s="2" t="n">
+        <v>46019</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -1548,143 +1598,119 @@
       <c r="AI12" t="inlineStr"/>
       <c r="AJ12" t="inlineStr"/>
       <c r="AK12" t="inlineStr"/>
-      <c r="AL12" t="inlineStr">
-        <is>
-          <t>Aagaaz</t>
-        </is>
-      </c>
+      <c r="AL12" t="inlineStr"/>
       <c r="AM12" t="n">
         <v>1</v>
       </c>
-      <c r="AN12" t="inlineStr"/>
+      <c r="AN12" t="inlineStr">
+        <is>
+          <t>Gender Leger</t>
+        </is>
+      </c>
       <c r="AO12" t="n">
         <v>68</v>
       </c>
-      <c r="AP12" t="inlineStr"/>
+      <c r="AP12" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
       <c r="AQ12" t="n">
         <v>48</v>
       </c>
       <c r="AR12" t="inlineStr"/>
-      <c r="AS12" t="inlineStr"/>
-      <c r="AT12" t="inlineStr"/>
+      <c r="AS12" t="inlineStr">
+        <is>
+          <t>43 x 19 mm</t>
+        </is>
+      </c>
+      <c r="AT12" t="inlineStr">
+        <is>
+          <t>48 x 22 mm</t>
+        </is>
+      </c>
       <c r="AU12" t="inlineStr"/>
-      <c r="AV12" t="inlineStr"/>
-      <c r="AW12" t="inlineStr"/>
+      <c r="AV12" t="inlineStr">
+        <is>
+          <t>Acetabulum and iliac wing appear normal.
+Femoral head appears normal and cartilagenous.
+Central ossific nucleus not visualised in femoral head on either side.
+No joint effusion.
+No intramusclar fluid collection.
+Right angle Alpha - 61
+Beta - 56
+Left angle Alpha - 62
+Beta - 55
+No obvious e/o developmental dysplasia of hip.</t>
+        </is>
+      </c>
+      <c r="AW12" t="inlineStr">
+        <is>
+          <t>;
+Normal study. .</t>
+        </is>
+      </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>2025-12-28</t>
-        </is>
+      <c r="A13" s="2" t="n">
+        <v>46019</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Complete Blood Picture (CBP)</t>
-        </is>
-      </c>
-      <c r="C13" t="n">
-        <v>11.3</v>
-      </c>
-      <c r="D13" t="n">
-        <v>3.78</v>
-      </c>
-      <c r="E13" t="n">
-        <v>10.84</v>
-      </c>
-      <c r="F13" t="n">
-        <v>486</v>
-      </c>
+          <t>Ultrasound Report</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
       <c r="G13" t="inlineStr"/>
       <c r="H13" t="inlineStr"/>
-      <c r="I13" t="n">
-        <v>13</v>
-      </c>
-      <c r="J13" t="n">
-        <v>9</v>
-      </c>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
       <c r="K13" t="inlineStr"/>
       <c r="L13" t="inlineStr"/>
       <c r="M13" t="inlineStr"/>
-      <c r="N13" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="O13" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="P13" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="Q13" t="n">
-        <v>34</v>
-      </c>
-      <c r="R13" t="n">
-        <v>27</v>
-      </c>
-      <c r="S13" t="n">
-        <v>360</v>
-      </c>
-      <c r="T13" t="n">
-        <v>6.5</v>
-      </c>
-      <c r="U13" t="n">
-        <v>46</v>
-      </c>
-      <c r="V13" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="W13" t="n">
-        <v>2.4</v>
-      </c>
+      <c r="N13" t="inlineStr"/>
+      <c r="O13" t="inlineStr"/>
+      <c r="P13" t="inlineStr"/>
+      <c r="Q13" t="inlineStr"/>
+      <c r="R13" t="inlineStr"/>
+      <c r="S13" t="inlineStr"/>
+      <c r="T13" t="inlineStr"/>
+      <c r="U13" t="inlineStr"/>
+      <c r="V13" t="inlineStr"/>
+      <c r="W13" t="inlineStr"/>
       <c r="X13" t="inlineStr"/>
-      <c r="Y13" t="n">
-        <v>78</v>
-      </c>
-      <c r="Z13" t="n">
-        <v>25.4</v>
-      </c>
-      <c r="AA13" t="n">
-        <v>32.6</v>
-      </c>
-      <c r="AB13" t="n">
-        <v>12.7</v>
-      </c>
-      <c r="AC13" t="n">
-        <v>8.199999999999999</v>
-      </c>
-      <c r="AD13" t="n">
-        <v>3</v>
-      </c>
-      <c r="AE13" t="n">
-        <v>4</v>
-      </c>
-      <c r="AF13" t="n">
-        <v>2.98</v>
-      </c>
-      <c r="AG13" t="n">
-        <v>26</v>
-      </c>
-      <c r="AH13" t="n">
-        <v>70</v>
-      </c>
-      <c r="AI13" t="n">
-        <v>2</v>
-      </c>
-      <c r="AJ13" t="n">
-        <v>2</v>
-      </c>
+      <c r="Y13" t="inlineStr"/>
+      <c r="Z13" t="inlineStr"/>
+      <c r="AA13" t="inlineStr"/>
+      <c r="AB13" t="inlineStr"/>
+      <c r="AC13" t="inlineStr"/>
+      <c r="AD13" t="inlineStr"/>
+      <c r="AE13" t="inlineStr"/>
+      <c r="AF13" t="inlineStr"/>
+      <c r="AG13" t="inlineStr"/>
+      <c r="AH13" t="inlineStr"/>
+      <c r="AI13" t="inlineStr"/>
+      <c r="AJ13" t="inlineStr"/>
       <c r="AK13" t="inlineStr"/>
       <c r="AL13" t="inlineStr">
         <is>
-          <t>KASHV</t>
+          <t>Aagaaz</t>
         </is>
       </c>
       <c r="AM13" t="n">
         <v>1</v>
       </c>
       <c r="AN13" t="inlineStr"/>
-      <c r="AO13" t="inlineStr"/>
+      <c r="AO13" t="n">
+        <v>68</v>
+      </c>
       <c r="AP13" t="inlineStr"/>
-      <c r="AQ13" t="inlineStr"/>
+      <c r="AQ13" t="n">
+        <v>48</v>
+      </c>
       <c r="AR13" t="inlineStr"/>
       <c r="AS13" t="inlineStr"/>
       <c r="AT13" t="inlineStr"/>
@@ -1693,10 +1719,8 @@
       <c r="AW13" t="inlineStr"/>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>2025-12-28</t>
-        </is>
+      <c r="A14" s="2" t="n">
+        <v>46019</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -1814,10 +1838,8 @@
       <c r="AW14" t="inlineStr"/>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>2025-12-28</t>
-        </is>
+      <c r="A15" s="2" t="n">
+        <v>46019</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -1935,114 +1957,58 @@
       <c r="AW15" t="inlineStr"/>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>2025-12-28</t>
-        </is>
+      <c r="A16" s="2" t="n">
+        <v>46019</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Complete Blood Picture (CBP)</t>
-        </is>
-      </c>
-      <c r="C16" t="n">
-        <v>11.3</v>
-      </c>
-      <c r="D16" t="n">
-        <v>3.78</v>
-      </c>
-      <c r="E16" t="n">
-        <v>10.84</v>
-      </c>
-      <c r="F16" t="n">
-        <v>486</v>
-      </c>
+          <t>Thyroid Test</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="inlineStr"/>
       <c r="G16" t="inlineStr"/>
       <c r="H16" t="inlineStr"/>
-      <c r="I16" t="n">
-        <v>13</v>
-      </c>
-      <c r="J16" t="n">
-        <v>9</v>
-      </c>
+      <c r="I16" t="inlineStr"/>
+      <c r="J16" t="inlineStr"/>
       <c r="K16" t="inlineStr"/>
       <c r="L16" t="inlineStr"/>
       <c r="M16" t="inlineStr"/>
-      <c r="N16" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="O16" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="P16" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="Q16" t="n">
-        <v>34</v>
-      </c>
-      <c r="R16" t="n">
-        <v>27</v>
-      </c>
-      <c r="S16" t="n">
-        <v>360</v>
-      </c>
-      <c r="T16" t="n">
-        <v>6.5</v>
-      </c>
-      <c r="U16" t="n">
-        <v>46</v>
-      </c>
-      <c r="V16" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="W16" t="n">
-        <v>2.4</v>
-      </c>
+      <c r="N16" t="inlineStr"/>
+      <c r="O16" t="inlineStr"/>
+      <c r="P16" t="inlineStr"/>
+      <c r="Q16" t="inlineStr"/>
+      <c r="R16" t="inlineStr"/>
+      <c r="S16" t="inlineStr"/>
+      <c r="T16" t="inlineStr"/>
+      <c r="U16" t="inlineStr"/>
+      <c r="V16" t="inlineStr"/>
+      <c r="W16" t="inlineStr"/>
       <c r="X16" t="inlineStr"/>
-      <c r="Y16" t="n">
-        <v>78</v>
-      </c>
-      <c r="Z16" t="n">
-        <v>25.4</v>
-      </c>
-      <c r="AA16" t="n">
-        <v>32.6</v>
-      </c>
-      <c r="AB16" t="n">
-        <v>12.7</v>
-      </c>
-      <c r="AC16" t="n">
-        <v>8.199999999999999</v>
-      </c>
+      <c r="Y16" t="inlineStr"/>
+      <c r="Z16" t="inlineStr"/>
+      <c r="AA16" t="inlineStr"/>
+      <c r="AB16" t="inlineStr"/>
+      <c r="AC16" t="inlineStr"/>
       <c r="AD16" t="n">
-        <v>3</v>
+        <v>176.2</v>
       </c>
       <c r="AE16" t="n">
-        <v>4</v>
+        <v>10.9</v>
       </c>
       <c r="AF16" t="n">
         <v>2.98</v>
       </c>
-      <c r="AG16" t="n">
-        <v>26</v>
-      </c>
-      <c r="AH16" t="n">
-        <v>70</v>
-      </c>
-      <c r="AI16" t="n">
-        <v>2</v>
-      </c>
-      <c r="AJ16" t="n">
-        <v>2</v>
-      </c>
+      <c r="AG16" t="inlineStr"/>
+      <c r="AH16" t="inlineStr"/>
+      <c r="AI16" t="inlineStr"/>
+      <c r="AJ16" t="inlineStr"/>
       <c r="AK16" t="inlineStr"/>
-      <c r="AL16" t="inlineStr">
-        <is>
-          <t>KASHV</t>
-        </is>
-      </c>
+      <c r="AL16" t="inlineStr"/>
       <c r="AM16" t="n">
-        <v>1</v>
+        <v>90</v>
       </c>
       <c r="AN16" t="inlineStr"/>
       <c r="AO16" t="inlineStr"/>
@@ -2056,14 +2022,12 @@
       <c r="AW16" t="inlineStr"/>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>2025-12-29</t>
-        </is>
+      <c r="A17" s="2" t="n">
+        <v>46019</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Ultrasound Report</t>
+          <t>Complete Blood Picture (CBP)</t>
         </is>
       </c>
       <c r="C17" t="n">
@@ -2166,30 +2130,149 @@
         <v>1</v>
       </c>
       <c r="AN17" t="inlineStr"/>
-      <c r="AO17" t="n">
+      <c r="AO17" t="inlineStr"/>
+      <c r="AP17" t="inlineStr"/>
+      <c r="AQ17" t="inlineStr"/>
+      <c r="AR17" t="inlineStr"/>
+      <c r="AS17" t="inlineStr"/>
+      <c r="AT17" t="inlineStr"/>
+      <c r="AU17" t="inlineStr"/>
+      <c r="AV17" t="inlineStr"/>
+      <c r="AW17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="n">
+        <v>46020</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Ultrasound Report</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>11.3</v>
+      </c>
+      <c r="D18" t="n">
+        <v>3.78</v>
+      </c>
+      <c r="E18" t="n">
+        <v>10.84</v>
+      </c>
+      <c r="F18" t="n">
+        <v>486</v>
+      </c>
+      <c r="G18" t="inlineStr"/>
+      <c r="H18" t="inlineStr"/>
+      <c r="I18" t="n">
+        <v>13</v>
+      </c>
+      <c r="J18" t="n">
+        <v>9</v>
+      </c>
+      <c r="K18" t="inlineStr"/>
+      <c r="L18" t="inlineStr"/>
+      <c r="M18" t="inlineStr"/>
+      <c r="N18" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="O18" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="P18" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>34</v>
+      </c>
+      <c r="R18" t="n">
+        <v>27</v>
+      </c>
+      <c r="S18" t="n">
+        <v>360</v>
+      </c>
+      <c r="T18" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="U18" t="n">
+        <v>46</v>
+      </c>
+      <c r="V18" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="W18" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="X18" t="inlineStr"/>
+      <c r="Y18" t="n">
+        <v>78</v>
+      </c>
+      <c r="Z18" t="n">
+        <v>25.4</v>
+      </c>
+      <c r="AA18" t="n">
+        <v>32.6</v>
+      </c>
+      <c r="AB18" t="n">
+        <v>12.7</v>
+      </c>
+      <c r="AC18" t="n">
+        <v>8.199999999999999</v>
+      </c>
+      <c r="AD18" t="n">
+        <v>3</v>
+      </c>
+      <c r="AE18" t="n">
+        <v>4</v>
+      </c>
+      <c r="AF18" t="n">
+        <v>2.98</v>
+      </c>
+      <c r="AG18" t="n">
+        <v>26</v>
+      </c>
+      <c r="AH18" t="n">
+        <v>70</v>
+      </c>
+      <c r="AI18" t="n">
+        <v>2</v>
+      </c>
+      <c r="AJ18" t="n">
+        <v>2</v>
+      </c>
+      <c r="AK18" t="inlineStr"/>
+      <c r="AL18" t="inlineStr">
+        <is>
+          <t>KASHV</t>
+        </is>
+      </c>
+      <c r="AM18" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN18" t="inlineStr"/>
+      <c r="AO18" t="n">
         <v>68</v>
       </c>
-      <c r="AP17" t="inlineStr">
+      <c r="AP18" t="inlineStr">
         <is>
           <t>Normal</t>
         </is>
       </c>
-      <c r="AQ17" t="n">
+      <c r="AQ18" t="n">
         <v>48</v>
       </c>
-      <c r="AR17" t="inlineStr"/>
-      <c r="AS17" t="inlineStr">
+      <c r="AR18" t="inlineStr"/>
+      <c r="AS18" t="inlineStr">
         <is>
           <t>43 x 19 mm</t>
         </is>
       </c>
-      <c r="AT17" t="inlineStr">
+      <c r="AT18" t="inlineStr">
         <is>
           <t>48 x 22 mm</t>
         </is>
       </c>
-      <c r="AU17" t="inlineStr"/>
-      <c r="AV17" t="inlineStr">
+      <c r="AU18" t="inlineStr"/>
+      <c r="AV18" t="inlineStr">
         <is>
           <t>Acetabulum and iliac wing appear normal.
 Femoral head appears normal and cartilagenous.
@@ -2203,143 +2286,20 @@
 No obvious e/o developmental dysplasia of hip.</t>
         </is>
       </c>
-      <c r="AW17" t="inlineStr">
+      <c r="AW18" t="inlineStr">
         <is>
           <t>;
 Normal study. .</t>
         </is>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>2025-12-29</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
+    <row r="19">
+      <c r="A19" s="2" t="n">
+        <v>46020</v>
+      </c>
+      <c r="B19" t="inlineStr">
         <is>
           <t>Liver Function Test (LFT)</t>
-        </is>
-      </c>
-      <c r="C18" t="n">
-        <v>11.3</v>
-      </c>
-      <c r="D18" t="n">
-        <v>3.78</v>
-      </c>
-      <c r="E18" t="n">
-        <v>10.84</v>
-      </c>
-      <c r="F18" t="n">
-        <v>486</v>
-      </c>
-      <c r="G18" t="inlineStr"/>
-      <c r="H18" t="inlineStr"/>
-      <c r="I18" t="n">
-        <v>13</v>
-      </c>
-      <c r="J18" t="n">
-        <v>9</v>
-      </c>
-      <c r="K18" t="inlineStr"/>
-      <c r="L18" t="inlineStr"/>
-      <c r="M18" t="inlineStr"/>
-      <c r="N18" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="O18" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="P18" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="Q18" t="n">
-        <v>34</v>
-      </c>
-      <c r="R18" t="n">
-        <v>27</v>
-      </c>
-      <c r="S18" t="n">
-        <v>360</v>
-      </c>
-      <c r="T18" t="n">
-        <v>6.5</v>
-      </c>
-      <c r="U18" t="n">
-        <v>46</v>
-      </c>
-      <c r="V18" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="W18" t="n">
-        <v>2.4</v>
-      </c>
-      <c r="X18" t="inlineStr"/>
-      <c r="Y18" t="n">
-        <v>78</v>
-      </c>
-      <c r="Z18" t="n">
-        <v>25.4</v>
-      </c>
-      <c r="AA18" t="n">
-        <v>32.6</v>
-      </c>
-      <c r="AB18" t="n">
-        <v>12.7</v>
-      </c>
-      <c r="AC18" t="n">
-        <v>8.199999999999999</v>
-      </c>
-      <c r="AD18" t="n">
-        <v>3</v>
-      </c>
-      <c r="AE18" t="n">
-        <v>4</v>
-      </c>
-      <c r="AF18" t="n">
-        <v>2.98</v>
-      </c>
-      <c r="AG18" t="n">
-        <v>26</v>
-      </c>
-      <c r="AH18" t="n">
-        <v>70</v>
-      </c>
-      <c r="AI18" t="n">
-        <v>2</v>
-      </c>
-      <c r="AJ18" t="n">
-        <v>2</v>
-      </c>
-      <c r="AK18" t="inlineStr"/>
-      <c r="AL18" t="inlineStr">
-        <is>
-          <t>KASHV</t>
-        </is>
-      </c>
-      <c r="AM18" t="n">
-        <v>1</v>
-      </c>
-      <c r="AN18" t="inlineStr"/>
-      <c r="AO18" t="inlineStr"/>
-      <c r="AP18" t="inlineStr"/>
-      <c r="AQ18" t="inlineStr"/>
-      <c r="AR18" t="inlineStr"/>
-      <c r="AS18" t="inlineStr"/>
-      <c r="AT18" t="inlineStr"/>
-      <c r="AU18" t="inlineStr"/>
-      <c r="AV18" t="inlineStr"/>
-      <c r="AW18" t="inlineStr"/>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>2025-12-29</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>Complete Blood Picture (CBP)</t>
         </is>
       </c>
       <c r="C19" t="n">
@@ -2438,10 +2398,8 @@
           <t>KASHV</t>
         </is>
       </c>
-      <c r="AM19" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="AM19" t="n">
+        <v>1</v>
       </c>
       <c r="AN19" t="inlineStr"/>
       <c r="AO19" t="inlineStr"/>
@@ -2454,6 +2412,385 @@
       <c r="AV19" t="inlineStr"/>
       <c r="AW19" t="inlineStr"/>
     </row>
+    <row r="20">
+      <c r="A20" s="2" t="n">
+        <v>46020</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Complete Blood Picture (CBP)</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>11.3</v>
+      </c>
+      <c r="D20" t="n">
+        <v>3.78</v>
+      </c>
+      <c r="E20" t="n">
+        <v>10.84</v>
+      </c>
+      <c r="F20" t="n">
+        <v>486</v>
+      </c>
+      <c r="G20" t="inlineStr"/>
+      <c r="H20" t="inlineStr"/>
+      <c r="I20" t="n">
+        <v>13</v>
+      </c>
+      <c r="J20" t="n">
+        <v>9</v>
+      </c>
+      <c r="K20" t="inlineStr"/>
+      <c r="L20" t="inlineStr"/>
+      <c r="M20" t="inlineStr"/>
+      <c r="N20" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="O20" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="P20" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>34</v>
+      </c>
+      <c r="R20" t="n">
+        <v>27</v>
+      </c>
+      <c r="S20" t="n">
+        <v>360</v>
+      </c>
+      <c r="T20" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="U20" t="n">
+        <v>46</v>
+      </c>
+      <c r="V20" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="W20" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="X20" t="inlineStr"/>
+      <c r="Y20" t="n">
+        <v>78</v>
+      </c>
+      <c r="Z20" t="n">
+        <v>25.4</v>
+      </c>
+      <c r="AA20" t="n">
+        <v>32.6</v>
+      </c>
+      <c r="AB20" t="n">
+        <v>12.7</v>
+      </c>
+      <c r="AC20" t="n">
+        <v>8.199999999999999</v>
+      </c>
+      <c r="AD20" t="n">
+        <v>3</v>
+      </c>
+      <c r="AE20" t="n">
+        <v>4</v>
+      </c>
+      <c r="AF20" t="n">
+        <v>2.98</v>
+      </c>
+      <c r="AG20" t="n">
+        <v>26</v>
+      </c>
+      <c r="AH20" t="n">
+        <v>70</v>
+      </c>
+      <c r="AI20" t="n">
+        <v>2</v>
+      </c>
+      <c r="AJ20" t="n">
+        <v>2</v>
+      </c>
+      <c r="AK20" t="inlineStr"/>
+      <c r="AL20" t="inlineStr">
+        <is>
+          <t>KASHV</t>
+        </is>
+      </c>
+      <c r="AM20" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN20" t="inlineStr"/>
+      <c r="AO20" t="inlineStr"/>
+      <c r="AP20" t="inlineStr"/>
+      <c r="AQ20" t="inlineStr"/>
+      <c r="AR20" t="inlineStr"/>
+      <c r="AS20" t="inlineStr"/>
+      <c r="AT20" t="inlineStr"/>
+      <c r="AU20" t="inlineStr"/>
+      <c r="AV20" t="inlineStr"/>
+      <c r="AW20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="2" t="n">
+        <v>46023</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Complete Blood Picture (CBP)</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>10.3</v>
+      </c>
+      <c r="D21" t="n">
+        <v>3.78</v>
+      </c>
+      <c r="E21" t="n">
+        <v>10.84</v>
+      </c>
+      <c r="F21" t="n">
+        <v>486</v>
+      </c>
+      <c r="G21" t="inlineStr"/>
+      <c r="H21" t="inlineStr"/>
+      <c r="I21" t="inlineStr"/>
+      <c r="J21" t="inlineStr"/>
+      <c r="K21" t="inlineStr"/>
+      <c r="L21" t="inlineStr"/>
+      <c r="M21" t="inlineStr"/>
+      <c r="N21" t="inlineStr"/>
+      <c r="O21" t="inlineStr"/>
+      <c r="P21" t="inlineStr"/>
+      <c r="Q21" t="inlineStr"/>
+      <c r="R21" t="inlineStr"/>
+      <c r="S21" t="inlineStr"/>
+      <c r="T21" t="inlineStr"/>
+      <c r="U21" t="inlineStr"/>
+      <c r="V21" t="inlineStr"/>
+      <c r="W21" t="inlineStr"/>
+      <c r="X21" t="inlineStr"/>
+      <c r="Y21" t="n">
+        <v>78.59999999999999</v>
+      </c>
+      <c r="Z21" t="inlineStr"/>
+      <c r="AA21" t="inlineStr"/>
+      <c r="AB21" t="inlineStr"/>
+      <c r="AC21" t="inlineStr"/>
+      <c r="AD21" t="inlineStr"/>
+      <c r="AE21" t="inlineStr"/>
+      <c r="AF21" t="inlineStr"/>
+      <c r="AG21" t="n">
+        <v>22.1</v>
+      </c>
+      <c r="AH21" t="n">
+        <v>66.09999999999999</v>
+      </c>
+      <c r="AI21" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="AJ21" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="AK21" t="inlineStr"/>
+      <c r="AL21" t="inlineStr">
+        <is>
+          <t>BirthRight
+Hospital</t>
+        </is>
+      </c>
+      <c r="AM21" t="n">
+        <v>42</v>
+      </c>
+      <c r="AN21" t="inlineStr"/>
+      <c r="AO21" t="inlineStr"/>
+      <c r="AP21" t="inlineStr"/>
+      <c r="AQ21" t="inlineStr"/>
+      <c r="AR21" t="inlineStr"/>
+      <c r="AS21" t="inlineStr"/>
+      <c r="AT21" t="inlineStr"/>
+      <c r="AU21" t="inlineStr"/>
+      <c r="AV21" t="inlineStr"/>
+      <c r="AW21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="n">
+        <v>46023</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Liver Function Test (LFT)</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>11.3</v>
+      </c>
+      <c r="D22" t="inlineStr"/>
+      <c r="E22" t="inlineStr"/>
+      <c r="F22" t="n">
+        <v>416</v>
+      </c>
+      <c r="G22" t="inlineStr"/>
+      <c r="H22" t="inlineStr"/>
+      <c r="I22" t="n">
+        <v>13</v>
+      </c>
+      <c r="J22" t="n">
+        <v>9</v>
+      </c>
+      <c r="K22" t="inlineStr"/>
+      <c r="L22" t="inlineStr"/>
+      <c r="M22" t="inlineStr"/>
+      <c r="N22" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="O22" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="P22" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="Q22" t="n">
+        <v>34</v>
+      </c>
+      <c r="R22" t="n">
+        <v>27</v>
+      </c>
+      <c r="S22" t="inlineStr"/>
+      <c r="T22" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="U22" t="n">
+        <v>46</v>
+      </c>
+      <c r="V22" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="W22" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="X22" t="inlineStr"/>
+      <c r="Y22" t="n">
+        <v>78</v>
+      </c>
+      <c r="Z22" t="n">
+        <v>25.4</v>
+      </c>
+      <c r="AA22" t="n">
+        <v>32.6</v>
+      </c>
+      <c r="AB22" t="n">
+        <v>12.7</v>
+      </c>
+      <c r="AC22" t="n">
+        <v>8.199999999999999</v>
+      </c>
+      <c r="AD22" t="inlineStr"/>
+      <c r="AE22" t="inlineStr"/>
+      <c r="AF22" t="inlineStr"/>
+      <c r="AG22" t="n">
+        <v>26</v>
+      </c>
+      <c r="AH22" t="n">
+        <v>70</v>
+      </c>
+      <c r="AI22" t="n">
+        <v>2</v>
+      </c>
+      <c r="AJ22" t="n">
+        <v>2</v>
+      </c>
+      <c r="AK22" t="inlineStr"/>
+      <c r="AL22" t="inlineStr">
+        <is>
+          <t>KASHV</t>
+        </is>
+      </c>
+      <c r="AM22" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN22" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="AO22" t="inlineStr"/>
+      <c r="AP22" t="inlineStr"/>
+      <c r="AQ22" t="inlineStr"/>
+      <c r="AR22" t="inlineStr"/>
+      <c r="AS22" t="inlineStr"/>
+      <c r="AT22" t="inlineStr"/>
+      <c r="AU22" t="inlineStr"/>
+      <c r="AV22" t="inlineStr"/>
+      <c r="AW22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="2" t="n">
+        <v>46023</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Thyroid Test</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr"/>
+      <c r="D23" t="inlineStr"/>
+      <c r="E23" t="inlineStr"/>
+      <c r="F23" t="inlineStr"/>
+      <c r="G23" t="inlineStr"/>
+      <c r="H23" t="inlineStr"/>
+      <c r="I23" t="inlineStr"/>
+      <c r="J23" t="inlineStr"/>
+      <c r="K23" t="inlineStr"/>
+      <c r="L23" t="inlineStr"/>
+      <c r="M23" t="inlineStr"/>
+      <c r="N23" t="inlineStr"/>
+      <c r="O23" t="inlineStr"/>
+      <c r="P23" t="inlineStr"/>
+      <c r="Q23" t="inlineStr"/>
+      <c r="R23" t="inlineStr"/>
+      <c r="S23" t="inlineStr"/>
+      <c r="T23" t="inlineStr"/>
+      <c r="U23" t="inlineStr"/>
+      <c r="V23" t="inlineStr"/>
+      <c r="W23" t="inlineStr"/>
+      <c r="X23" t="inlineStr"/>
+      <c r="Y23" t="inlineStr"/>
+      <c r="Z23" t="inlineStr"/>
+      <c r="AA23" t="inlineStr"/>
+      <c r="AB23" t="inlineStr"/>
+      <c r="AC23" t="inlineStr"/>
+      <c r="AD23" t="n">
+        <v>3</v>
+      </c>
+      <c r="AE23" t="n">
+        <v>4</v>
+      </c>
+      <c r="AF23" t="n">
+        <v>2.98</v>
+      </c>
+      <c r="AG23" t="inlineStr"/>
+      <c r="AH23" t="inlineStr"/>
+      <c r="AI23" t="inlineStr"/>
+      <c r="AJ23" t="inlineStr"/>
+      <c r="AK23" t="inlineStr"/>
+      <c r="AL23" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="AM23" t="inlineStr"/>
+      <c r="AN23" t="inlineStr"/>
+      <c r="AO23" t="inlineStr"/>
+      <c r="AP23" t="inlineStr"/>
+      <c r="AQ23" t="inlineStr"/>
+      <c r="AR23" t="inlineStr"/>
+      <c r="AS23" t="inlineStr"/>
+      <c r="AT23" t="inlineStr"/>
+      <c r="AU23" t="inlineStr"/>
+      <c r="AV23" t="inlineStr"/>
+      <c r="AW23" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Family feature, longitudnal analysis
</commit_message>
<xml_diff>
--- a/data/reports/test_reports.xlsx
+++ b/data/reports/test_reports.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AW23"/>
+  <dimension ref="A1:AW24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2791,6 +2791,129 @@
       <c r="AV23" t="inlineStr"/>
       <c r="AW23" t="inlineStr"/>
     </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2025-09-08</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Liver Function Test (LFT)</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>11.3</v>
+      </c>
+      <c r="D24" t="n">
+        <v>3.78</v>
+      </c>
+      <c r="E24" t="n">
+        <v>10.84</v>
+      </c>
+      <c r="F24" t="n">
+        <v>486</v>
+      </c>
+      <c r="G24" t="inlineStr"/>
+      <c r="H24" t="inlineStr"/>
+      <c r="I24" t="n">
+        <v>13</v>
+      </c>
+      <c r="J24" t="n">
+        <v>9</v>
+      </c>
+      <c r="K24" t="inlineStr"/>
+      <c r="L24" t="inlineStr"/>
+      <c r="M24" t="inlineStr"/>
+      <c r="N24" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="O24" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="P24" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="Q24" t="n">
+        <v>34</v>
+      </c>
+      <c r="R24" t="n">
+        <v>27</v>
+      </c>
+      <c r="S24" t="n">
+        <v>360</v>
+      </c>
+      <c r="T24" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="U24" t="n">
+        <v>46</v>
+      </c>
+      <c r="V24" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="W24" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="X24" t="inlineStr"/>
+      <c r="Y24" t="n">
+        <v>78</v>
+      </c>
+      <c r="Z24" t="n">
+        <v>25.4</v>
+      </c>
+      <c r="AA24" t="n">
+        <v>32.6</v>
+      </c>
+      <c r="AB24" t="n">
+        <v>12.7</v>
+      </c>
+      <c r="AC24" t="n">
+        <v>8.199999999999999</v>
+      </c>
+      <c r="AD24" t="n">
+        <v>3</v>
+      </c>
+      <c r="AE24" t="n">
+        <v>4</v>
+      </c>
+      <c r="AF24" t="n">
+        <v>2.98</v>
+      </c>
+      <c r="AG24" t="n">
+        <v>26</v>
+      </c>
+      <c r="AH24" t="n">
+        <v>70</v>
+      </c>
+      <c r="AI24" t="n">
+        <v>2</v>
+      </c>
+      <c r="AJ24" t="n">
+        <v>2</v>
+      </c>
+      <c r="AK24" t="inlineStr"/>
+      <c r="AL24" t="inlineStr">
+        <is>
+          <t>KASHV</t>
+        </is>
+      </c>
+      <c r="AM24" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AN24" t="inlineStr"/>
+      <c r="AO24" t="inlineStr"/>
+      <c r="AP24" t="inlineStr"/>
+      <c r="AQ24" t="inlineStr"/>
+      <c r="AR24" t="inlineStr"/>
+      <c r="AS24" t="inlineStr"/>
+      <c r="AT24" t="inlineStr"/>
+      <c r="AU24" t="inlineStr"/>
+      <c r="AV24" t="inlineStr"/>
+      <c r="AW24" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>